<commit_message>
update patient and adress + example
</commit_message>
<xml_diff>
--- a/StructureDefinition-be-address.xlsx
+++ b/StructureDefinition-be-address.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AM$14</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AM$21</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="187">
   <si>
     <t>Path</t>
   </si>
@@ -228,6 +228,22 @@
 ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}</t>
   </si>
   <si>
+    <t>language</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension {language}
+</t>
+  </si>
+  <si>
+    <t>Human Language for the item</t>
+  </si>
+  <si>
+    <t>The Human Language of the item.</t>
+  </si>
+  <si>
+    <t>This is used where an item may repeat to indicate the language of each repeat.</t>
+  </si>
+  <si>
     <t>Address.use</t>
   </si>
   <si>
@@ -349,6 +365,78 @@
     <t>street</t>
   </si>
   <si>
+    <t>Address.line.id</t>
+  </si>
+  <si>
+    <t>xml:id (or equivalent in JSON)</t>
+  </si>
+  <si>
+    <t>unique id for the element within a resource (for internal references)</t>
+  </si>
+  <si>
+    <t>Address.line.extension</t>
+  </si>
+  <si>
+    <t>Extension</t>
+  </si>
+  <si>
+    <t>An Extension</t>
+  </si>
+  <si>
+    <t>streetName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension {iso21090-ADXP-streetName}
+</t>
+  </si>
+  <si>
+    <t>streetName.</t>
+  </si>
+  <si>
+    <t>ADXP[partType=STR]</t>
+  </si>
+  <si>
+    <t>houseNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension {iso21090-ADXP-houseNumber}
+</t>
+  </si>
+  <si>
+    <t>The number of a building, house or lot alongside the street. Also known as "primary street number". This does not number the street but rather the building.</t>
+  </si>
+  <si>
+    <t>ADXP[partType=BNR]</t>
+  </si>
+  <si>
+    <t>postBox</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension {iso21090-ADXP-postBox}
+</t>
+  </si>
+  <si>
+    <t>A numbered box located in a post station.</t>
+  </si>
+  <si>
+    <t>ADXP[partType=POB]</t>
+  </si>
+  <si>
+    <t>Address.line.value</t>
+  </si>
+  <si>
+    <t>Primitive value for string</t>
+  </si>
+  <si>
+    <t>The actual value</t>
+  </si>
+  <si>
+    <t>1048576</t>
+  </si>
+  <si>
+    <t>string.value</t>
+  </si>
+  <si>
     <t>Address.city</t>
   </si>
   <si>
@@ -461,7 +549,8 @@
     <t>Country (e.g. can be ISO 3166 2 or 3 letter code)</t>
   </si>
   <si>
-    <t>Country - a nation as commonly understood or generally accepted.</t>
+    <t>Country - a nation as commonly understood or generally accepted. Concerning the codification of the country, the FHIR specification defines its country field as a string and suggests using a ISO 3166 2 or 3 letter codes. 
+As that 2-letter format is also the standard in a KMEHR address, it is hence RECOMMENDED to codify the country in the same way as in KMEHR.</t>
   </si>
   <si>
     <t>ISO 3166 3 letter codes can be used in place of a human readable country name.</t>
@@ -656,7 +745,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AM14"/>
+  <dimension ref="A1:AM21"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -665,8 +754,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="18.8125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="11.1328125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="21.2890625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="13.8125" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="12.3828125" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="5.8984375" customWidth="true" bestFit="true" hidden="true"/>
     <col min="5" max="5" width="4.69921875" customWidth="true" bestFit="true"/>
@@ -1158,9 +1247,11 @@
     </row>
     <row r="5" hidden="true">
       <c r="A5" t="s" s="2">
+        <v>57</v>
+      </c>
+      <c r="B5" t="s" s="2">
         <v>68</v>
       </c>
-      <c r="B5" s="2"/>
       <c r="C5" t="s" s="2">
         <v>40</v>
       </c>
@@ -1175,26 +1266,24 @@
         <v>40</v>
       </c>
       <c r="H5" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I5" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="J5" t="s" s="2">
         <v>69</v>
       </c>
-      <c r="I5" t="s" s="2">
-        <v>69</v>
-      </c>
-      <c r="J5" t="s" s="2">
+      <c r="K5" t="s" s="2">
         <v>70</v>
       </c>
-      <c r="K5" t="s" s="2">
+      <c r="L5" t="s" s="2">
         <v>71</v>
       </c>
-      <c r="L5" t="s" s="2">
+      <c r="M5" t="s" s="2">
         <v>72</v>
       </c>
-      <c r="M5" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="N5" t="s" s="2">
-        <v>74</v>
-      </c>
+      <c r="N5" s="2"/>
       <c r="O5" t="s" s="2">
         <v>40</v>
       </c>
@@ -1206,7 +1295,7 @@
         <v>40</v>
       </c>
       <c r="S5" t="s" s="2">
-        <v>75</v>
+        <v>40</v>
       </c>
       <c r="T5" t="s" s="2">
         <v>40</v>
@@ -1218,13 +1307,13 @@
         <v>40</v>
       </c>
       <c r="W5" t="s" s="2">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="X5" t="s" s="2">
-        <v>77</v>
+        <v>40</v>
       </c>
       <c r="Y5" t="s" s="2">
-        <v>78</v>
+        <v>40</v>
       </c>
       <c r="Z5" t="s" s="2">
         <v>40</v>
@@ -1242,28 +1331,28 @@
         <v>40</v>
       </c>
       <c r="AE5" t="s" s="2">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="AF5" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG5" t="s" s="2">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="AH5" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI5" t="s" s="2">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="AJ5" t="s" s="2">
-        <v>79</v>
+        <v>40</v>
       </c>
       <c r="AK5" t="s" s="2">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="AL5" t="s" s="2">
-        <v>81</v>
+        <v>40</v>
       </c>
       <c r="AM5" t="s" s="2">
         <v>40</v>
@@ -1271,7 +1360,7 @@
     </row>
     <row r="6" hidden="true">
       <c r="A6" t="s" s="2">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" t="s" s="2">
@@ -1288,24 +1377,26 @@
         <v>40</v>
       </c>
       <c r="H6" t="s" s="2">
-        <v>40</v>
+        <v>74</v>
       </c>
       <c r="I6" t="s" s="2">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="J6" t="s" s="2">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="K6" t="s" s="2">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="L6" t="s" s="2">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="M6" t="s" s="2">
-        <v>85</v>
-      </c>
-      <c r="N6" s="2"/>
+        <v>78</v>
+      </c>
+      <c r="N6" t="s" s="2">
+        <v>79</v>
+      </c>
       <c r="O6" t="s" s="2">
         <v>40</v>
       </c>
@@ -1317,7 +1408,7 @@
         <v>40</v>
       </c>
       <c r="S6" t="s" s="2">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="T6" t="s" s="2">
         <v>40</v>
@@ -1329,13 +1420,13 @@
         <v>40</v>
       </c>
       <c r="W6" t="s" s="2">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="X6" t="s" s="2">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="Y6" t="s" s="2">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="Z6" t="s" s="2">
         <v>40</v>
@@ -1353,7 +1444,7 @@
         <v>40</v>
       </c>
       <c r="AE6" t="s" s="2">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="AF6" t="s" s="2">
         <v>41</v>
@@ -1368,21 +1459,21 @@
         <v>47</v>
       </c>
       <c r="AJ6" t="s" s="2">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="AK6" t="s" s="2">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="AL6" t="s" s="2">
-        <v>40</v>
+        <v>86</v>
       </c>
       <c r="AM6" t="s" s="2">
-        <v>90</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" hidden="true">
       <c r="A7" t="s" s="2">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" t="s" s="2">
@@ -1402,23 +1493,21 @@
         <v>40</v>
       </c>
       <c r="I7" t="s" s="2">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="J7" t="s" s="2">
-        <v>52</v>
+        <v>75</v>
       </c>
       <c r="K7" t="s" s="2">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="L7" t="s" s="2">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="M7" t="s" s="2">
-        <v>94</v>
-      </c>
-      <c r="N7" t="s" s="2">
-        <v>95</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="N7" s="2"/>
       <c r="O7" t="s" s="2">
         <v>40</v>
       </c>
@@ -1430,7 +1519,7 @@
         <v>40</v>
       </c>
       <c r="S7" t="s" s="2">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="T7" t="s" s="2">
         <v>40</v>
@@ -1442,13 +1531,13 @@
         <v>40</v>
       </c>
       <c r="W7" t="s" s="2">
-        <v>40</v>
+        <v>81</v>
       </c>
       <c r="X7" t="s" s="2">
-        <v>40</v>
+        <v>92</v>
       </c>
       <c r="Y7" t="s" s="2">
-        <v>40</v>
+        <v>93</v>
       </c>
       <c r="Z7" t="s" s="2">
         <v>40</v>
@@ -1466,7 +1555,7 @@
         <v>40</v>
       </c>
       <c r="AE7" t="s" s="2">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="AF7" t="s" s="2">
         <v>41</v>
@@ -1481,21 +1570,21 @@
         <v>47</v>
       </c>
       <c r="AJ7" t="s" s="2">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="AK7" t="s" s="2">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="AL7" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM7" t="s" s="2">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" hidden="true">
       <c r="A8" t="s" s="2">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" t="s" s="2">
@@ -1506,7 +1595,7 @@
         <v>41</v>
       </c>
       <c r="F8" t="s" s="2">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="G8" t="s" s="2">
         <v>40</v>
@@ -1515,19 +1604,23 @@
         <v>40</v>
       </c>
       <c r="I8" t="s" s="2">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="J8" t="s" s="2">
         <v>52</v>
       </c>
       <c r="K8" t="s" s="2">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="L8" t="s" s="2">
-        <v>102</v>
-      </c>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
+        <v>98</v>
+      </c>
+      <c r="M8" t="s" s="2">
+        <v>99</v>
+      </c>
+      <c r="N8" t="s" s="2">
+        <v>100</v>
+      </c>
       <c r="O8" t="s" s="2">
         <v>40</v>
       </c>
@@ -1539,7 +1632,7 @@
         <v>40</v>
       </c>
       <c r="S8" t="s" s="2">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="T8" t="s" s="2">
         <v>40</v>
@@ -1575,13 +1668,13 @@
         <v>40</v>
       </c>
       <c r="AE8" t="s" s="2">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="AF8" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG8" t="s" s="2">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="AH8" t="s" s="2">
         <v>40</v>
@@ -1590,32 +1683,32 @@
         <v>47</v>
       </c>
       <c r="AJ8" t="s" s="2">
+        <v>102</v>
+      </c>
+      <c r="AK8" t="s" s="2">
+        <v>103</v>
+      </c>
+      <c r="AL8" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM8" t="s" s="2">
         <v>104</v>
-      </c>
-      <c r="AK8" t="s" s="2">
-        <v>105</v>
-      </c>
-      <c r="AL8" t="s" s="2">
-        <v>106</v>
-      </c>
-      <c r="AM8" t="s" s="2">
-        <v>107</v>
       </c>
     </row>
     <row r="9" hidden="true">
       <c r="A9" t="s" s="2">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s" s="2">
-        <v>109</v>
+        <v>40</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F9" t="s" s="2">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="G9" t="s" s="2">
         <v>40</v>
@@ -1624,16 +1717,16 @@
         <v>40</v>
       </c>
       <c r="I9" t="s" s="2">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="J9" t="s" s="2">
         <v>52</v>
       </c>
       <c r="K9" t="s" s="2">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="L9" t="s" s="2">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
@@ -1648,7 +1741,7 @@
         <v>40</v>
       </c>
       <c r="S9" t="s" s="2">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="T9" t="s" s="2">
         <v>40</v>
@@ -1684,13 +1777,13 @@
         <v>40</v>
       </c>
       <c r="AE9" t="s" s="2">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="AF9" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG9" t="s" s="2">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="AH9" t="s" s="2">
         <v>40</v>
@@ -1699,25 +1792,25 @@
         <v>47</v>
       </c>
       <c r="AJ9" t="s" s="2">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="AK9" t="s" s="2">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="AL9" t="s" s="2">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="AM9" t="s" s="2">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10" hidden="true">
       <c r="A10" t="s" s="2">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" t="s" s="2">
-        <v>118</v>
+        <v>40</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" t="s" s="2">
@@ -1733,20 +1826,18 @@
         <v>40</v>
       </c>
       <c r="I10" t="s" s="2">
-        <v>69</v>
+        <v>40</v>
       </c>
       <c r="J10" t="s" s="2">
         <v>52</v>
       </c>
       <c r="K10" t="s" s="2">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="L10" t="s" s="2">
-        <v>120</v>
-      </c>
-      <c r="M10" t="s" s="2">
-        <v>121</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="M10" s="2"/>
       <c r="N10" s="2"/>
       <c r="O10" t="s" s="2">
         <v>40</v>
@@ -1759,7 +1850,7 @@
         <v>40</v>
       </c>
       <c r="S10" t="s" s="2">
-        <v>122</v>
+        <v>40</v>
       </c>
       <c r="T10" t="s" s="2">
         <v>40</v>
@@ -1795,7 +1886,7 @@
         <v>40</v>
       </c>
       <c r="AE10" t="s" s="2">
-        <v>117</v>
+        <v>55</v>
       </c>
       <c r="AF10" t="s" s="2">
         <v>41</v>
@@ -1807,13 +1898,13 @@
         <v>40</v>
       </c>
       <c r="AI10" t="s" s="2">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="AJ10" t="s" s="2">
-        <v>123</v>
+        <v>40</v>
       </c>
       <c r="AK10" t="s" s="2">
-        <v>124</v>
+        <v>40</v>
       </c>
       <c r="AL10" t="s" s="2">
         <v>40</v>
@@ -1824,18 +1915,18 @@
     </row>
     <row r="11" hidden="true">
       <c r="A11" t="s" s="2">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" t="s" s="2">
-        <v>126</v>
+        <v>40</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F11" t="s" s="2">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="G11" t="s" s="2">
         <v>40</v>
@@ -1844,16 +1935,16 @@
         <v>40</v>
       </c>
       <c r="I11" t="s" s="2">
-        <v>69</v>
+        <v>40</v>
       </c>
       <c r="J11" t="s" s="2">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="K11" t="s" s="2">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="L11" t="s" s="2">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
@@ -1892,59 +1983,59 @@
         <v>40</v>
       </c>
       <c r="AA11" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB11" t="s" s="2">
-        <v>40</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="AB11" s="2"/>
       <c r="AC11" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AD11" t="s" s="2">
-        <v>40</v>
+        <v>65</v>
       </c>
       <c r="AE11" t="s" s="2">
-        <v>125</v>
+        <v>66</v>
       </c>
       <c r="AF11" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG11" t="s" s="2">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="AH11" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI11" t="s" s="2">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="AJ11" t="s" s="2">
-        <v>129</v>
+        <v>40</v>
       </c>
       <c r="AK11" t="s" s="2">
-        <v>130</v>
+        <v>40</v>
       </c>
       <c r="AL11" t="s" s="2">
-        <v>131</v>
+        <v>40</v>
       </c>
       <c r="AM11" t="s" s="2">
-        <v>132</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" hidden="true">
       <c r="A12" t="s" s="2">
-        <v>133</v>
-      </c>
-      <c r="B12" s="2"/>
+        <v>116</v>
+      </c>
+      <c r="B12" t="s" s="2">
+        <v>119</v>
+      </c>
       <c r="C12" t="s" s="2">
-        <v>134</v>
+        <v>40</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F12" t="s" s="2">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="G12" t="s" s="2">
         <v>40</v>
@@ -1953,16 +2044,16 @@
         <v>40</v>
       </c>
       <c r="I12" t="s" s="2">
-        <v>69</v>
+        <v>40</v>
       </c>
       <c r="J12" t="s" s="2">
-        <v>52</v>
+        <v>120</v>
       </c>
       <c r="K12" t="s" s="2">
-        <v>135</v>
+        <v>119</v>
       </c>
       <c r="L12" t="s" s="2">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
@@ -1977,7 +2068,7 @@
         <v>40</v>
       </c>
       <c r="S12" t="s" s="2">
-        <v>137</v>
+        <v>40</v>
       </c>
       <c r="T12" t="s" s="2">
         <v>40</v>
@@ -2013,38 +2104,40 @@
         <v>40</v>
       </c>
       <c r="AE12" t="s" s="2">
-        <v>133</v>
+        <v>66</v>
       </c>
       <c r="AF12" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG12" t="s" s="2">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="AH12" t="s" s="2">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="AI12" t="s" s="2">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="AJ12" t="s" s="2">
-        <v>138</v>
+        <v>40</v>
       </c>
       <c r="AK12" t="s" s="2">
-        <v>139</v>
+        <v>122</v>
       </c>
       <c r="AL12" t="s" s="2">
-        <v>140</v>
+        <v>40</v>
       </c>
       <c r="AM12" t="s" s="2">
-        <v>141</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" hidden="true">
       <c r="A13" t="s" s="2">
-        <v>142</v>
-      </c>
-      <c r="B13" s="2"/>
+        <v>116</v>
+      </c>
+      <c r="B13" t="s" s="2">
+        <v>123</v>
+      </c>
       <c r="C13" t="s" s="2">
         <v>40</v>
       </c>
@@ -2053,7 +2146,7 @@
         <v>41</v>
       </c>
       <c r="F13" t="s" s="2">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="G13" t="s" s="2">
         <v>40</v>
@@ -2062,20 +2155,18 @@
         <v>40</v>
       </c>
       <c r="I13" t="s" s="2">
-        <v>69</v>
+        <v>40</v>
       </c>
       <c r="J13" t="s" s="2">
-        <v>52</v>
+        <v>124</v>
       </c>
       <c r="K13" t="s" s="2">
-        <v>143</v>
+        <v>123</v>
       </c>
       <c r="L13" t="s" s="2">
-        <v>144</v>
-      </c>
-      <c r="M13" t="s" s="2">
-        <v>145</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="M13" s="2"/>
       <c r="N13" s="2"/>
       <c r="O13" t="s" s="2">
         <v>40</v>
@@ -2124,38 +2215,40 @@
         <v>40</v>
       </c>
       <c r="AE13" t="s" s="2">
-        <v>142</v>
+        <v>66</v>
       </c>
       <c r="AF13" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG13" t="s" s="2">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="AH13" t="s" s="2">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="AI13" t="s" s="2">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="AJ13" t="s" s="2">
-        <v>146</v>
+        <v>40</v>
       </c>
       <c r="AK13" t="s" s="2">
-        <v>147</v>
+        <v>126</v>
       </c>
       <c r="AL13" t="s" s="2">
-        <v>148</v>
+        <v>40</v>
       </c>
       <c r="AM13" t="s" s="2">
-        <v>149</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" hidden="true">
       <c r="A14" t="s" s="2">
-        <v>150</v>
-      </c>
-      <c r="B14" s="2"/>
+        <v>116</v>
+      </c>
+      <c r="B14" t="s" s="2">
+        <v>127</v>
+      </c>
       <c r="C14" t="s" s="2">
         <v>40</v>
       </c>
@@ -2164,7 +2257,7 @@
         <v>41</v>
       </c>
       <c r="F14" t="s" s="2">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="G14" t="s" s="2">
         <v>40</v>
@@ -2173,21 +2266,19 @@
         <v>40</v>
       </c>
       <c r="I14" t="s" s="2">
-        <v>69</v>
+        <v>40</v>
       </c>
       <c r="J14" t="s" s="2">
-        <v>151</v>
+        <v>128</v>
       </c>
       <c r="K14" t="s" s="2">
-        <v>152</v>
+        <v>127</v>
       </c>
       <c r="L14" t="s" s="2">
-        <v>153</v>
+        <v>129</v>
       </c>
       <c r="M14" s="2"/>
-      <c r="N14" t="s" s="2">
-        <v>154</v>
-      </c>
+      <c r="N14" s="2"/>
       <c r="O14" t="s" s="2">
         <v>40</v>
       </c>
@@ -2199,71 +2290,840 @@
         <v>40</v>
       </c>
       <c r="S14" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T14" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U14" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V14" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W14" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X14" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y14" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z14" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA14" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB14" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC14" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD14" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE14" t="s" s="2">
+        <v>66</v>
+      </c>
+      <c r="AF14" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG14" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AH14" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="AI14" t="s" s="2">
+        <v>67</v>
+      </c>
+      <c r="AJ14" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK14" t="s" s="2">
+        <v>130</v>
+      </c>
+      <c r="AL14" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM14" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" hidden="true">
+      <c r="A15" t="s" s="2">
+        <v>131</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F15" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="G15" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H15" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I15" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="J15" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="K15" t="s" s="2">
+        <v>132</v>
+      </c>
+      <c r="L15" t="s" s="2">
+        <v>133</v>
+      </c>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P15" s="2"/>
+      <c r="Q15" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R15" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S15" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T15" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U15" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V15" t="s" s="2">
+        <v>134</v>
+      </c>
+      <c r="W15" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X15" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y15" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z15" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA15" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB15" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC15" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD15" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE15" t="s" s="2">
+        <v>135</v>
+      </c>
+      <c r="AF15" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG15" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH15" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI15" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ15" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK15" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AL15" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM15" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" hidden="true">
+      <c r="A16" t="s" s="2">
+        <v>136</v>
+      </c>
+      <c r="B16" s="2"/>
+      <c r="C16" t="s" s="2">
+        <v>137</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F16" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="G16" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H16" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I16" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="J16" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="K16" t="s" s="2">
+        <v>138</v>
+      </c>
+      <c r="L16" t="s" s="2">
+        <v>139</v>
+      </c>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P16" s="2"/>
+      <c r="Q16" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R16" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S16" t="s" s="2">
+        <v>140</v>
+      </c>
+      <c r="T16" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U16" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V16" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W16" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X16" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y16" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z16" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA16" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB16" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC16" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD16" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE16" t="s" s="2">
+        <v>136</v>
+      </c>
+      <c r="AF16" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG16" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH16" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI16" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="AJ16" t="s" s="2">
+        <v>141</v>
+      </c>
+      <c r="AK16" t="s" s="2">
+        <v>142</v>
+      </c>
+      <c r="AL16" t="s" s="2">
+        <v>143</v>
+      </c>
+      <c r="AM16" t="s" s="2">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="17" hidden="true">
+      <c r="A17" t="s" s="2">
+        <v>145</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" t="s" s="2">
+        <v>146</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F17" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="G17" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H17" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I17" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="J17" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="K17" t="s" s="2">
+        <v>147</v>
+      </c>
+      <c r="L17" t="s" s="2">
+        <v>148</v>
+      </c>
+      <c r="M17" t="s" s="2">
+        <v>149</v>
+      </c>
+      <c r="N17" s="2"/>
+      <c r="O17" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P17" s="2"/>
+      <c r="Q17" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R17" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S17" t="s" s="2">
+        <v>150</v>
+      </c>
+      <c r="T17" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U17" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V17" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W17" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X17" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y17" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z17" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA17" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB17" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC17" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD17" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE17" t="s" s="2">
+        <v>145</v>
+      </c>
+      <c r="AF17" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG17" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH17" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI17" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="AJ17" t="s" s="2">
+        <v>151</v>
+      </c>
+      <c r="AK17" t="s" s="2">
+        <v>152</v>
+      </c>
+      <c r="AL17" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM17" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" hidden="true">
+      <c r="A18" t="s" s="2">
+        <v>153</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" t="s" s="2">
+        <v>154</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F18" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="G18" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H18" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I18" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="J18" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="K18" t="s" s="2">
         <v>155</v>
       </c>
-      <c r="T14" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="U14" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="V14" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="W14" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="X14" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="Y14" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="Z14" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AA14" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB14" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AC14" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AD14" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AE14" t="s" s="2">
-        <v>150</v>
-      </c>
-      <c r="AF14" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG14" t="s" s="2">
+      <c r="L18" t="s" s="2">
+        <v>156</v>
+      </c>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P18" s="2"/>
+      <c r="Q18" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R18" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S18" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T18" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U18" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V18" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W18" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X18" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y18" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z18" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA18" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB18" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC18" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD18" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE18" t="s" s="2">
+        <v>153</v>
+      </c>
+      <c r="AF18" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG18" t="s" s="2">
         <v>51</v>
       </c>
-      <c r="AH14" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI14" t="s" s="2">
+      <c r="AH18" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI18" t="s" s="2">
         <v>47</v>
       </c>
-      <c r="AJ14" t="s" s="2">
-        <v>156</v>
-      </c>
-      <c r="AK14" t="s" s="2">
+      <c r="AJ18" t="s" s="2">
         <v>157</v>
       </c>
-      <c r="AL14" t="s" s="2">
+      <c r="AK18" t="s" s="2">
         <v>158</v>
       </c>
-      <c r="AM14" t="s" s="2">
+      <c r="AL18" t="s" s="2">
+        <v>159</v>
+      </c>
+      <c r="AM18" t="s" s="2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="19" hidden="true">
+      <c r="A19" t="s" s="2">
+        <v>161</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" t="s" s="2">
+        <v>162</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F19" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="G19" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H19" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I19" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="J19" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="K19" t="s" s="2">
+        <v>163</v>
+      </c>
+      <c r="L19" t="s" s="2">
+        <v>164</v>
+      </c>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P19" s="2"/>
+      <c r="Q19" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R19" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S19" t="s" s="2">
+        <v>165</v>
+      </c>
+      <c r="T19" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U19" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V19" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W19" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X19" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y19" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z19" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA19" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB19" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC19" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD19" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE19" t="s" s="2">
+        <v>161</v>
+      </c>
+      <c r="AF19" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG19" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH19" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI19" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="AJ19" t="s" s="2">
+        <v>166</v>
+      </c>
+      <c r="AK19" t="s" s="2">
+        <v>167</v>
+      </c>
+      <c r="AL19" t="s" s="2">
+        <v>168</v>
+      </c>
+      <c r="AM19" t="s" s="2">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="20" hidden="true">
+      <c r="A20" t="s" s="2">
+        <v>170</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="E20" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F20" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="G20" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H20" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I20" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="J20" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="K20" t="s" s="2">
+        <v>171</v>
+      </c>
+      <c r="L20" t="s" s="2">
+        <v>172</v>
+      </c>
+      <c r="M20" t="s" s="2">
+        <v>173</v>
+      </c>
+      <c r="N20" s="2"/>
+      <c r="O20" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P20" s="2"/>
+      <c r="Q20" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R20" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S20" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T20" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U20" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V20" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W20" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X20" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y20" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z20" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA20" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB20" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC20" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD20" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE20" t="s" s="2">
+        <v>170</v>
+      </c>
+      <c r="AF20" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG20" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH20" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI20" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="AJ20" t="s" s="2">
+        <v>174</v>
+      </c>
+      <c r="AK20" t="s" s="2">
+        <v>175</v>
+      </c>
+      <c r="AL20" t="s" s="2">
+        <v>176</v>
+      </c>
+      <c r="AM20" t="s" s="2">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="21" hidden="true">
+      <c r="A21" t="s" s="2">
+        <v>178</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="E21" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F21" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="G21" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H21" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I21" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="J21" t="s" s="2">
+        <v>179</v>
+      </c>
+      <c r="K21" t="s" s="2">
+        <v>180</v>
+      </c>
+      <c r="L21" t="s" s="2">
+        <v>181</v>
+      </c>
+      <c r="M21" s="2"/>
+      <c r="N21" t="s" s="2">
+        <v>182</v>
+      </c>
+      <c r="O21" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P21" s="2"/>
+      <c r="Q21" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R21" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S21" t="s" s="2">
+        <v>183</v>
+      </c>
+      <c r="T21" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U21" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V21" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W21" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X21" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y21" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z21" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA21" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB21" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC21" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD21" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE21" t="s" s="2">
+        <v>178</v>
+      </c>
+      <c r="AF21" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG21" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH21" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI21" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="AJ21" t="s" s="2">
+        <v>184</v>
+      </c>
+      <c r="AK21" t="s" s="2">
+        <v>185</v>
+      </c>
+      <c r="AL21" t="s" s="2">
+        <v>186</v>
+      </c>
+      <c r="AM21" t="s" s="2">
         <v>40</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AM14">
+  <autoFilter ref="A1:AM21">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -2273,7 +3133,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI13">
+  <conditionalFormatting sqref="A2:AI20">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>

<commit_message>
update organization and address + example
</commit_message>
<xml_diff>
--- a/StructureDefinition-be-address.xlsx
+++ b/StructureDefinition-be-address.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AM$21</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AM$36</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1246" uniqueCount="206">
   <si>
     <t>Path</t>
   </si>
@@ -396,6 +396,59 @@
     <t>ADXP[partType=STR]</t>
   </si>
   <si>
+    <t>Address.line.extension.id</t>
+  </si>
+  <si>
+    <t>Address.line.extension.extension</t>
+  </si>
+  <si>
+    <t>Address.line.extension.url</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uri
+</t>
+  </si>
+  <si>
+    <t>identifies the meaning of the extension</t>
+  </si>
+  <si>
+    <t>Source of the definition for the extension code - a logical name or a URL.</t>
+  </si>
+  <si>
+    <t>The definition may point directly to a computable or human-readable definition of the extensibility codes, or it may be a logical URI as declared in some other specification. The definition SHALL be a URI for the Structure Definition defining the extension.</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/StructureDefinition/iso21090-ADXP-streetName</t>
+  </si>
+  <si>
+    <t>Extension.url</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Address.line.extension.value[x]</t>
+  </si>
+  <si>
+    <t>Value of extension</t>
+  </si>
+  <si>
+    <t>Value of extension - must be one of a constrained set of the data types (see [Extensibility](http://hl7.org/fhir/extensibility.html) for a list).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">type:$this}
+</t>
+  </si>
+  <si>
+    <t>closed</t>
+  </si>
+  <si>
+    <t>Extension.value[x]</t>
+  </si>
+  <si>
+    <t>valueString</t>
+  </si>
+  <si>
     <t>houseNumber</t>
   </si>
   <si>
@@ -409,6 +462,9 @@
     <t>ADXP[partType=BNR]</t>
   </si>
   <si>
+    <t>http://hl7.org/fhir/StructureDefinition/iso21090-ADXP-houseNumber</t>
+  </si>
+  <si>
     <t>postBox</t>
   </si>
   <si>
@@ -420,6 +476,9 @@
   </si>
   <si>
     <t>ADXP[partType=POB]</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/StructureDefinition/iso21090-ADXP-postBox</t>
   </si>
   <si>
     <t>Address.line.value</t>
@@ -745,7 +804,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AM21"/>
+  <dimension ref="A1:AM36"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -754,7 +813,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="21.2890625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="30.5625" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="13.8125" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="12.3828125" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="5.8984375" customWidth="true" bestFit="true" hidden="true"/>
@@ -2133,11 +2192,9 @@
     </row>
     <row r="13" hidden="true">
       <c r="A13" t="s" s="2">
-        <v>116</v>
-      </c>
-      <c r="B13" t="s" s="2">
         <v>123</v>
       </c>
+      <c r="B13" s="2"/>
       <c r="C13" t="s" s="2">
         <v>40</v>
       </c>
@@ -2146,7 +2203,7 @@
         <v>41</v>
       </c>
       <c r="F13" t="s" s="2">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="G13" t="s" s="2">
         <v>40</v>
@@ -2158,13 +2215,13 @@
         <v>40</v>
       </c>
       <c r="J13" t="s" s="2">
-        <v>124</v>
+        <v>52</v>
       </c>
       <c r="K13" t="s" s="2">
-        <v>123</v>
+        <v>53</v>
       </c>
       <c r="L13" t="s" s="2">
-        <v>125</v>
+        <v>54</v>
       </c>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
@@ -2215,25 +2272,25 @@
         <v>40</v>
       </c>
       <c r="AE13" t="s" s="2">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="AF13" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG13" t="s" s="2">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="AH13" t="s" s="2">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="AI13" t="s" s="2">
-        <v>67</v>
+        <v>40</v>
       </c>
       <c r="AJ13" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AK13" t="s" s="2">
-        <v>126</v>
+        <v>56</v>
       </c>
       <c r="AL13" t="s" s="2">
         <v>40</v>
@@ -2244,11 +2301,9 @@
     </row>
     <row r="14" hidden="true">
       <c r="A14" t="s" s="2">
-        <v>116</v>
-      </c>
-      <c r="B14" t="s" s="2">
-        <v>127</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="B14" s="2"/>
       <c r="C14" t="s" s="2">
         <v>40</v>
       </c>
@@ -2257,7 +2312,7 @@
         <v>41</v>
       </c>
       <c r="F14" t="s" s="2">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G14" t="s" s="2">
         <v>40</v>
@@ -2269,13 +2324,13 @@
         <v>40</v>
       </c>
       <c r="J14" t="s" s="2">
-        <v>128</v>
+        <v>59</v>
       </c>
       <c r="K14" t="s" s="2">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="L14" t="s" s="2">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
@@ -2314,16 +2369,16 @@
         <v>40</v>
       </c>
       <c r="AA14" t="s" s="2">
-        <v>40</v>
+        <v>63</v>
       </c>
       <c r="AB14" t="s" s="2">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="AC14" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AD14" t="s" s="2">
-        <v>40</v>
+        <v>65</v>
       </c>
       <c r="AE14" t="s" s="2">
         <v>66</v>
@@ -2335,7 +2390,7 @@
         <v>42</v>
       </c>
       <c r="AH14" t="s" s="2">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="AI14" t="s" s="2">
         <v>67</v>
@@ -2344,7 +2399,7 @@
         <v>40</v>
       </c>
       <c r="AK14" t="s" s="2">
-        <v>130</v>
+        <v>40</v>
       </c>
       <c r="AL14" t="s" s="2">
         <v>40</v>
@@ -2355,7 +2410,7 @@
     </row>
     <row r="15" hidden="true">
       <c r="A15" t="s" s="2">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s" s="2">
@@ -2363,7 +2418,7 @@
       </c>
       <c r="D15" s="2"/>
       <c r="E15" t="s" s="2">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="F15" t="s" s="2">
         <v>51</v>
@@ -2378,22 +2433,24 @@
         <v>40</v>
       </c>
       <c r="J15" t="s" s="2">
-        <v>52</v>
+        <v>126</v>
       </c>
       <c r="K15" t="s" s="2">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="L15" t="s" s="2">
-        <v>133</v>
-      </c>
-      <c r="M15" s="2"/>
+        <v>128</v>
+      </c>
+      <c r="M15" t="s" s="2">
+        <v>129</v>
+      </c>
       <c r="N15" s="2"/>
       <c r="O15" t="s" s="2">
         <v>40</v>
       </c>
       <c r="P15" s="2"/>
       <c r="Q15" t="s" s="2">
-        <v>40</v>
+        <v>130</v>
       </c>
       <c r="R15" t="s" s="2">
         <v>40</v>
@@ -2408,7 +2465,7 @@
         <v>40</v>
       </c>
       <c r="V15" t="s" s="2">
-        <v>134</v>
+        <v>40</v>
       </c>
       <c r="W15" t="s" s="2">
         <v>40</v>
@@ -2435,10 +2492,10 @@
         <v>40</v>
       </c>
       <c r="AE15" t="s" s="2">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="AF15" t="s" s="2">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="AG15" t="s" s="2">
         <v>51</v>
@@ -2453,7 +2510,7 @@
         <v>40</v>
       </c>
       <c r="AK15" t="s" s="2">
-        <v>40</v>
+        <v>132</v>
       </c>
       <c r="AL15" t="s" s="2">
         <v>40</v>
@@ -2464,15 +2521,15 @@
     </row>
     <row r="16" hidden="true">
       <c r="A16" t="s" s="2">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s" s="2">
-        <v>137</v>
+        <v>40</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" t="s" s="2">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="F16" t="s" s="2">
         <v>51</v>
@@ -2484,16 +2541,16 @@
         <v>40</v>
       </c>
       <c r="I16" t="s" s="2">
-        <v>74</v>
+        <v>40</v>
       </c>
       <c r="J16" t="s" s="2">
         <v>52</v>
       </c>
       <c r="K16" t="s" s="2">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="L16" t="s" s="2">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
@@ -2508,7 +2565,7 @@
         <v>40</v>
       </c>
       <c r="S16" t="s" s="2">
-        <v>140</v>
+        <v>40</v>
       </c>
       <c r="T16" t="s" s="2">
         <v>40</v>
@@ -2532,19 +2589,17 @@
         <v>40</v>
       </c>
       <c r="AA16" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB16" t="s" s="2">
-        <v>40</v>
-      </c>
+        <v>136</v>
+      </c>
+      <c r="AB16" s="2"/>
       <c r="AC16" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AD16" t="s" s="2">
-        <v>40</v>
+        <v>137</v>
       </c>
       <c r="AE16" t="s" s="2">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="AF16" t="s" s="2">
         <v>41</v>
@@ -2559,25 +2614,27 @@
         <v>47</v>
       </c>
       <c r="AJ16" t="s" s="2">
-        <v>141</v>
+        <v>40</v>
       </c>
       <c r="AK16" t="s" s="2">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="AL16" t="s" s="2">
-        <v>143</v>
+        <v>40</v>
       </c>
       <c r="AM16" t="s" s="2">
-        <v>144</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" hidden="true">
       <c r="A17" t="s" s="2">
-        <v>145</v>
-      </c>
-      <c r="B17" s="2"/>
+        <v>133</v>
+      </c>
+      <c r="B17" t="s" s="2">
+        <v>139</v>
+      </c>
       <c r="C17" t="s" s="2">
-        <v>146</v>
+        <v>40</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" t="s" s="2">
@@ -2593,20 +2650,18 @@
         <v>40</v>
       </c>
       <c r="I17" t="s" s="2">
-        <v>74</v>
+        <v>40</v>
       </c>
       <c r="J17" t="s" s="2">
         <v>52</v>
       </c>
       <c r="K17" t="s" s="2">
-        <v>147</v>
+        <v>134</v>
       </c>
       <c r="L17" t="s" s="2">
-        <v>148</v>
-      </c>
-      <c r="M17" t="s" s="2">
-        <v>149</v>
-      </c>
+        <v>135</v>
+      </c>
+      <c r="M17" s="2"/>
       <c r="N17" s="2"/>
       <c r="O17" t="s" s="2">
         <v>40</v>
@@ -2619,7 +2674,7 @@
         <v>40</v>
       </c>
       <c r="S17" t="s" s="2">
-        <v>150</v>
+        <v>40</v>
       </c>
       <c r="T17" t="s" s="2">
         <v>40</v>
@@ -2655,7 +2710,7 @@
         <v>40</v>
       </c>
       <c r="AE17" t="s" s="2">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="AF17" t="s" s="2">
         <v>41</v>
@@ -2670,10 +2725,10 @@
         <v>47</v>
       </c>
       <c r="AJ17" t="s" s="2">
-        <v>151</v>
+        <v>40</v>
       </c>
       <c r="AK17" t="s" s="2">
-        <v>152</v>
+        <v>132</v>
       </c>
       <c r="AL17" t="s" s="2">
         <v>40</v>
@@ -2684,18 +2739,20 @@
     </row>
     <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
-        <v>153</v>
-      </c>
-      <c r="B18" s="2"/>
+        <v>116</v>
+      </c>
+      <c r="B18" t="s" s="2">
+        <v>140</v>
+      </c>
       <c r="C18" t="s" s="2">
-        <v>154</v>
+        <v>40</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F18" t="s" s="2">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="G18" t="s" s="2">
         <v>40</v>
@@ -2704,16 +2761,16 @@
         <v>40</v>
       </c>
       <c r="I18" t="s" s="2">
-        <v>74</v>
+        <v>40</v>
       </c>
       <c r="J18" t="s" s="2">
-        <v>52</v>
+        <v>141</v>
       </c>
       <c r="K18" t="s" s="2">
-        <v>155</v>
+        <v>140</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
@@ -2764,40 +2821,40 @@
         <v>40</v>
       </c>
       <c r="AE18" t="s" s="2">
-        <v>153</v>
+        <v>66</v>
       </c>
       <c r="AF18" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG18" t="s" s="2">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="AH18" t="s" s="2">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="AI18" t="s" s="2">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="AJ18" t="s" s="2">
-        <v>157</v>
+        <v>40</v>
       </c>
       <c r="AK18" t="s" s="2">
-        <v>158</v>
+        <v>143</v>
       </c>
       <c r="AL18" t="s" s="2">
-        <v>159</v>
+        <v>40</v>
       </c>
       <c r="AM18" t="s" s="2">
-        <v>160</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>161</v>
+        <v>123</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
-        <v>162</v>
+        <v>40</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" t="s" s="2">
@@ -2813,16 +2870,16 @@
         <v>40</v>
       </c>
       <c r="I19" t="s" s="2">
-        <v>74</v>
+        <v>40</v>
       </c>
       <c r="J19" t="s" s="2">
         <v>52</v>
       </c>
       <c r="K19" t="s" s="2">
-        <v>163</v>
+        <v>53</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>164</v>
+        <v>54</v>
       </c>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
@@ -2837,7 +2894,7 @@
         <v>40</v>
       </c>
       <c r="S19" t="s" s="2">
-        <v>165</v>
+        <v>40</v>
       </c>
       <c r="T19" t="s" s="2">
         <v>40</v>
@@ -2873,7 +2930,7 @@
         <v>40</v>
       </c>
       <c r="AE19" t="s" s="2">
-        <v>161</v>
+        <v>55</v>
       </c>
       <c r="AF19" t="s" s="2">
         <v>41</v>
@@ -2885,24 +2942,24 @@
         <v>40</v>
       </c>
       <c r="AI19" t="s" s="2">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="AJ19" t="s" s="2">
-        <v>166</v>
+        <v>40</v>
       </c>
       <c r="AK19" t="s" s="2">
-        <v>167</v>
+        <v>56</v>
       </c>
       <c r="AL19" t="s" s="2">
-        <v>168</v>
+        <v>40</v>
       </c>
       <c r="AM19" t="s" s="2">
-        <v>169</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
-        <v>170</v>
+        <v>124</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s" s="2">
@@ -2913,7 +2970,7 @@
         <v>41</v>
       </c>
       <c r="F20" t="s" s="2">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="G20" t="s" s="2">
         <v>40</v>
@@ -2922,20 +2979,18 @@
         <v>40</v>
       </c>
       <c r="I20" t="s" s="2">
-        <v>74</v>
+        <v>40</v>
       </c>
       <c r="J20" t="s" s="2">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="K20" t="s" s="2">
-        <v>171</v>
+        <v>117</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>172</v>
-      </c>
-      <c r="M20" t="s" s="2">
-        <v>173</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="M20" s="2"/>
       <c r="N20" s="2"/>
       <c r="O20" t="s" s="2">
         <v>40</v>
@@ -2972,48 +3027,48 @@
         <v>40</v>
       </c>
       <c r="AA20" t="s" s="2">
-        <v>40</v>
+        <v>63</v>
       </c>
       <c r="AB20" t="s" s="2">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="AC20" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AD20" t="s" s="2">
-        <v>40</v>
+        <v>65</v>
       </c>
       <c r="AE20" t="s" s="2">
-        <v>170</v>
+        <v>66</v>
       </c>
       <c r="AF20" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG20" t="s" s="2">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="AH20" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI20" t="s" s="2">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="AJ20" t="s" s="2">
-        <v>174</v>
+        <v>40</v>
       </c>
       <c r="AK20" t="s" s="2">
-        <v>175</v>
+        <v>40</v>
       </c>
       <c r="AL20" t="s" s="2">
-        <v>176</v>
+        <v>40</v>
       </c>
       <c r="AM20" t="s" s="2">
-        <v>177</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>178</v>
+        <v>125</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s" s="2">
@@ -3021,7 +3076,7 @@
       </c>
       <c r="D21" s="2"/>
       <c r="E21" t="s" s="2">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="F21" t="s" s="2">
         <v>51</v>
@@ -3033,97 +3088,1742 @@
         <v>40</v>
       </c>
       <c r="I21" t="s" s="2">
-        <v>74</v>
+        <v>40</v>
       </c>
       <c r="J21" t="s" s="2">
-        <v>179</v>
+        <v>126</v>
       </c>
       <c r="K21" t="s" s="2">
-        <v>180</v>
+        <v>127</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>181</v>
-      </c>
-      <c r="M21" s="2"/>
-      <c r="N21" t="s" s="2">
-        <v>182</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="M21" t="s" s="2">
+        <v>129</v>
+      </c>
+      <c r="N21" s="2"/>
       <c r="O21" t="s" s="2">
         <v>40</v>
       </c>
       <c r="P21" s="2"/>
       <c r="Q21" t="s" s="2">
-        <v>40</v>
+        <v>144</v>
       </c>
       <c r="R21" t="s" s="2">
         <v>40</v>
       </c>
       <c r="S21" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T21" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U21" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V21" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W21" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X21" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y21" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z21" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA21" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB21" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC21" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD21" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE21" t="s" s="2">
+        <v>131</v>
+      </c>
+      <c r="AF21" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AG21" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH21" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI21" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ21" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK21" t="s" s="2">
+        <v>132</v>
+      </c>
+      <c r="AL21" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM21" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" hidden="true">
+      <c r="A22" t="s" s="2">
+        <v>133</v>
+      </c>
+      <c r="B22" s="2"/>
+      <c r="C22" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="D22" s="2"/>
+      <c r="E22" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="F22" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="G22" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H22" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I22" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="J22" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="K22" t="s" s="2">
+        <v>134</v>
+      </c>
+      <c r="L22" t="s" s="2">
+        <v>135</v>
+      </c>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+      <c r="O22" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P22" s="2"/>
+      <c r="Q22" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R22" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S22" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T22" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U22" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V22" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W22" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X22" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y22" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z22" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA22" t="s" s="2">
+        <v>136</v>
+      </c>
+      <c r="AB22" s="2"/>
+      <c r="AC22" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD22" t="s" s="2">
+        <v>137</v>
+      </c>
+      <c r="AE22" t="s" s="2">
+        <v>138</v>
+      </c>
+      <c r="AF22" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG22" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH22" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI22" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="AJ22" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK22" t="s" s="2">
+        <v>132</v>
+      </c>
+      <c r="AL22" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM22" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" hidden="true">
+      <c r="A23" t="s" s="2">
+        <v>133</v>
+      </c>
+      <c r="B23" t="s" s="2">
+        <v>139</v>
+      </c>
+      <c r="C23" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="D23" s="2"/>
+      <c r="E23" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F23" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="G23" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H23" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I23" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="J23" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="K23" t="s" s="2">
+        <v>134</v>
+      </c>
+      <c r="L23" t="s" s="2">
+        <v>135</v>
+      </c>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P23" s="2"/>
+      <c r="Q23" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R23" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S23" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T23" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U23" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V23" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W23" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X23" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y23" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z23" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA23" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB23" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC23" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD23" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE23" t="s" s="2">
+        <v>138</v>
+      </c>
+      <c r="AF23" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG23" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH23" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI23" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="AJ23" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK23" t="s" s="2">
+        <v>132</v>
+      </c>
+      <c r="AL23" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM23" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" hidden="true">
+      <c r="A24" t="s" s="2">
+        <v>116</v>
+      </c>
+      <c r="B24" t="s" s="2">
+        <v>145</v>
+      </c>
+      <c r="C24" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="D24" s="2"/>
+      <c r="E24" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F24" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="G24" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H24" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I24" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="J24" t="s" s="2">
+        <v>146</v>
+      </c>
+      <c r="K24" t="s" s="2">
+        <v>145</v>
+      </c>
+      <c r="L24" t="s" s="2">
+        <v>147</v>
+      </c>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P24" s="2"/>
+      <c r="Q24" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R24" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S24" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T24" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U24" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V24" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W24" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X24" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y24" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z24" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA24" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB24" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC24" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD24" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE24" t="s" s="2">
+        <v>66</v>
+      </c>
+      <c r="AF24" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG24" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AH24" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="AI24" t="s" s="2">
+        <v>67</v>
+      </c>
+      <c r="AJ24" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK24" t="s" s="2">
+        <v>148</v>
+      </c>
+      <c r="AL24" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM24" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" hidden="true">
+      <c r="A25" t="s" s="2">
+        <v>123</v>
+      </c>
+      <c r="B25" s="2"/>
+      <c r="C25" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="D25" s="2"/>
+      <c r="E25" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F25" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="G25" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H25" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I25" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="J25" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="K25" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="L25" t="s" s="2">
+        <v>54</v>
+      </c>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+      <c r="O25" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P25" s="2"/>
+      <c r="Q25" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R25" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S25" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T25" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U25" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V25" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W25" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X25" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y25" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z25" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA25" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB25" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC25" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD25" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE25" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="AF25" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG25" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH25" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI25" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ25" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK25" t="s" s="2">
+        <v>56</v>
+      </c>
+      <c r="AL25" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM25" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" hidden="true">
+      <c r="A26" t="s" s="2">
+        <v>124</v>
+      </c>
+      <c r="B26" s="2"/>
+      <c r="C26" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="D26" s="2"/>
+      <c r="E26" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F26" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="G26" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H26" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I26" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="J26" t="s" s="2">
+        <v>59</v>
+      </c>
+      <c r="K26" t="s" s="2">
+        <v>117</v>
+      </c>
+      <c r="L26" t="s" s="2">
+        <v>118</v>
+      </c>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+      <c r="O26" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P26" s="2"/>
+      <c r="Q26" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R26" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S26" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T26" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U26" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V26" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W26" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X26" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y26" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z26" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA26" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="AB26" t="s" s="2">
+        <v>64</v>
+      </c>
+      <c r="AC26" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD26" t="s" s="2">
+        <v>65</v>
+      </c>
+      <c r="AE26" t="s" s="2">
+        <v>66</v>
+      </c>
+      <c r="AF26" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG26" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AH26" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI26" t="s" s="2">
+        <v>67</v>
+      </c>
+      <c r="AJ26" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK26" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AL26" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM26" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" hidden="true">
+      <c r="A27" t="s" s="2">
+        <v>125</v>
+      </c>
+      <c r="B27" s="2"/>
+      <c r="C27" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="D27" s="2"/>
+      <c r="E27" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="F27" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="G27" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H27" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I27" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="J27" t="s" s="2">
+        <v>126</v>
+      </c>
+      <c r="K27" t="s" s="2">
+        <v>127</v>
+      </c>
+      <c r="L27" t="s" s="2">
+        <v>128</v>
+      </c>
+      <c r="M27" t="s" s="2">
+        <v>129</v>
+      </c>
+      <c r="N27" s="2"/>
+      <c r="O27" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P27" s="2"/>
+      <c r="Q27" t="s" s="2">
+        <v>149</v>
+      </c>
+      <c r="R27" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S27" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T27" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U27" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V27" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W27" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X27" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y27" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z27" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA27" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB27" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC27" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD27" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE27" t="s" s="2">
+        <v>131</v>
+      </c>
+      <c r="AF27" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AG27" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH27" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI27" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ27" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK27" t="s" s="2">
+        <v>132</v>
+      </c>
+      <c r="AL27" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM27" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" hidden="true">
+      <c r="A28" t="s" s="2">
+        <v>133</v>
+      </c>
+      <c r="B28" s="2"/>
+      <c r="C28" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="D28" s="2"/>
+      <c r="E28" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="F28" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="G28" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H28" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I28" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="J28" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="K28" t="s" s="2">
+        <v>134</v>
+      </c>
+      <c r="L28" t="s" s="2">
+        <v>135</v>
+      </c>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2"/>
+      <c r="O28" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P28" s="2"/>
+      <c r="Q28" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R28" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S28" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T28" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U28" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V28" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W28" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X28" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y28" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z28" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA28" t="s" s="2">
+        <v>136</v>
+      </c>
+      <c r="AB28" s="2"/>
+      <c r="AC28" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD28" t="s" s="2">
+        <v>137</v>
+      </c>
+      <c r="AE28" t="s" s="2">
+        <v>138</v>
+      </c>
+      <c r="AF28" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG28" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH28" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI28" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="AJ28" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK28" t="s" s="2">
+        <v>132</v>
+      </c>
+      <c r="AL28" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM28" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" hidden="true">
+      <c r="A29" t="s" s="2">
+        <v>133</v>
+      </c>
+      <c r="B29" t="s" s="2">
+        <v>139</v>
+      </c>
+      <c r="C29" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="D29" s="2"/>
+      <c r="E29" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F29" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="G29" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H29" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I29" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="J29" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="K29" t="s" s="2">
+        <v>134</v>
+      </c>
+      <c r="L29" t="s" s="2">
+        <v>135</v>
+      </c>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
+      <c r="O29" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P29" s="2"/>
+      <c r="Q29" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R29" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S29" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T29" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U29" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V29" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W29" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X29" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y29" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z29" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA29" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB29" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC29" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD29" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE29" t="s" s="2">
+        <v>138</v>
+      </c>
+      <c r="AF29" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG29" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH29" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI29" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="AJ29" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK29" t="s" s="2">
+        <v>132</v>
+      </c>
+      <c r="AL29" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM29" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" hidden="true">
+      <c r="A30" t="s" s="2">
+        <v>150</v>
+      </c>
+      <c r="B30" s="2"/>
+      <c r="C30" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="D30" s="2"/>
+      <c r="E30" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F30" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="G30" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H30" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I30" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="J30" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="K30" t="s" s="2">
+        <v>151</v>
+      </c>
+      <c r="L30" t="s" s="2">
+        <v>152</v>
+      </c>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
+      <c r="O30" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P30" s="2"/>
+      <c r="Q30" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R30" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S30" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T30" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U30" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V30" t="s" s="2">
+        <v>153</v>
+      </c>
+      <c r="W30" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X30" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y30" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z30" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA30" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB30" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC30" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD30" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE30" t="s" s="2">
+        <v>154</v>
+      </c>
+      <c r="AF30" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG30" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH30" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI30" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ30" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK30" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AL30" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM30" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" hidden="true">
+      <c r="A31" t="s" s="2">
+        <v>155</v>
+      </c>
+      <c r="B31" s="2"/>
+      <c r="C31" t="s" s="2">
+        <v>156</v>
+      </c>
+      <c r="D31" s="2"/>
+      <c r="E31" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F31" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="G31" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H31" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I31" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="J31" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="K31" t="s" s="2">
+        <v>157</v>
+      </c>
+      <c r="L31" t="s" s="2">
+        <v>158</v>
+      </c>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
+      <c r="O31" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P31" s="2"/>
+      <c r="Q31" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R31" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S31" t="s" s="2">
+        <v>159</v>
+      </c>
+      <c r="T31" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U31" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V31" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W31" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X31" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y31" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z31" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA31" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB31" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC31" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD31" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE31" t="s" s="2">
+        <v>155</v>
+      </c>
+      <c r="AF31" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG31" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH31" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI31" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="AJ31" t="s" s="2">
+        <v>160</v>
+      </c>
+      <c r="AK31" t="s" s="2">
+        <v>161</v>
+      </c>
+      <c r="AL31" t="s" s="2">
+        <v>162</v>
+      </c>
+      <c r="AM31" t="s" s="2">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="32" hidden="true">
+      <c r="A32" t="s" s="2">
+        <v>164</v>
+      </c>
+      <c r="B32" s="2"/>
+      <c r="C32" t="s" s="2">
+        <v>165</v>
+      </c>
+      <c r="D32" s="2"/>
+      <c r="E32" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F32" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="G32" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H32" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I32" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="J32" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="K32" t="s" s="2">
+        <v>166</v>
+      </c>
+      <c r="L32" t="s" s="2">
+        <v>167</v>
+      </c>
+      <c r="M32" t="s" s="2">
+        <v>168</v>
+      </c>
+      <c r="N32" s="2"/>
+      <c r="O32" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P32" s="2"/>
+      <c r="Q32" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R32" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S32" t="s" s="2">
+        <v>169</v>
+      </c>
+      <c r="T32" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U32" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V32" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W32" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X32" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y32" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z32" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA32" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB32" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC32" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD32" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE32" t="s" s="2">
+        <v>164</v>
+      </c>
+      <c r="AF32" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG32" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH32" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI32" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="AJ32" t="s" s="2">
+        <v>170</v>
+      </c>
+      <c r="AK32" t="s" s="2">
+        <v>171</v>
+      </c>
+      <c r="AL32" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM32" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" hidden="true">
+      <c r="A33" t="s" s="2">
+        <v>172</v>
+      </c>
+      <c r="B33" s="2"/>
+      <c r="C33" t="s" s="2">
+        <v>173</v>
+      </c>
+      <c r="D33" s="2"/>
+      <c r="E33" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F33" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="G33" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H33" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I33" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="J33" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="K33" t="s" s="2">
+        <v>174</v>
+      </c>
+      <c r="L33" t="s" s="2">
+        <v>175</v>
+      </c>
+      <c r="M33" s="2"/>
+      <c r="N33" s="2"/>
+      <c r="O33" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P33" s="2"/>
+      <c r="Q33" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R33" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S33" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T33" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U33" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V33" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W33" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X33" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y33" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z33" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA33" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB33" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC33" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD33" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE33" t="s" s="2">
+        <v>172</v>
+      </c>
+      <c r="AF33" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG33" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH33" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI33" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="AJ33" t="s" s="2">
+        <v>176</v>
+      </c>
+      <c r="AK33" t="s" s="2">
+        <v>177</v>
+      </c>
+      <c r="AL33" t="s" s="2">
+        <v>178</v>
+      </c>
+      <c r="AM33" t="s" s="2">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="34" hidden="true">
+      <c r="A34" t="s" s="2">
+        <v>180</v>
+      </c>
+      <c r="B34" s="2"/>
+      <c r="C34" t="s" s="2">
+        <v>181</v>
+      </c>
+      <c r="D34" s="2"/>
+      <c r="E34" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F34" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="G34" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H34" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I34" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="J34" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="K34" t="s" s="2">
+        <v>182</v>
+      </c>
+      <c r="L34" t="s" s="2">
         <v>183</v>
       </c>
-      <c r="T21" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="U21" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="V21" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="W21" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="X21" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="Y21" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="Z21" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AA21" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB21" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AC21" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AD21" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AE21" t="s" s="2">
-        <v>178</v>
-      </c>
-      <c r="AF21" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG21" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="AH21" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI21" t="s" s="2">
+      <c r="M34" s="2"/>
+      <c r="N34" s="2"/>
+      <c r="O34" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P34" s="2"/>
+      <c r="Q34" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R34" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S34" t="s" s="2">
+        <v>184</v>
+      </c>
+      <c r="T34" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U34" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V34" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W34" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X34" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y34" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z34" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA34" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB34" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC34" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD34" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE34" t="s" s="2">
+        <v>180</v>
+      </c>
+      <c r="AF34" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG34" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH34" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI34" t="s" s="2">
         <v>47</v>
       </c>
-      <c r="AJ21" t="s" s="2">
-        <v>184</v>
-      </c>
-      <c r="AK21" t="s" s="2">
+      <c r="AJ34" t="s" s="2">
         <v>185</v>
       </c>
-      <c r="AL21" t="s" s="2">
+      <c r="AK34" t="s" s="2">
         <v>186</v>
       </c>
-      <c r="AM21" t="s" s="2">
+      <c r="AL34" t="s" s="2">
+        <v>187</v>
+      </c>
+      <c r="AM34" t="s" s="2">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="35" hidden="true">
+      <c r="A35" t="s" s="2">
+        <v>189</v>
+      </c>
+      <c r="B35" s="2"/>
+      <c r="C35" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="D35" s="2"/>
+      <c r="E35" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F35" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="G35" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H35" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I35" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="J35" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="K35" t="s" s="2">
+        <v>190</v>
+      </c>
+      <c r="L35" t="s" s="2">
+        <v>191</v>
+      </c>
+      <c r="M35" t="s" s="2">
+        <v>192</v>
+      </c>
+      <c r="N35" s="2"/>
+      <c r="O35" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P35" s="2"/>
+      <c r="Q35" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R35" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S35" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T35" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U35" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V35" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W35" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X35" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y35" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z35" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA35" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB35" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC35" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD35" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE35" t="s" s="2">
+        <v>189</v>
+      </c>
+      <c r="AF35" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG35" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH35" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI35" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="AJ35" t="s" s="2">
+        <v>193</v>
+      </c>
+      <c r="AK35" t="s" s="2">
+        <v>194</v>
+      </c>
+      <c r="AL35" t="s" s="2">
+        <v>195</v>
+      </c>
+      <c r="AM35" t="s" s="2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="36" hidden="true">
+      <c r="A36" t="s" s="2">
+        <v>197</v>
+      </c>
+      <c r="B36" s="2"/>
+      <c r="C36" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="D36" s="2"/>
+      <c r="E36" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F36" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="G36" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H36" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I36" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="J36" t="s" s="2">
+        <v>198</v>
+      </c>
+      <c r="K36" t="s" s="2">
+        <v>199</v>
+      </c>
+      <c r="L36" t="s" s="2">
+        <v>200</v>
+      </c>
+      <c r="M36" s="2"/>
+      <c r="N36" t="s" s="2">
+        <v>201</v>
+      </c>
+      <c r="O36" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P36" s="2"/>
+      <c r="Q36" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R36" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S36" t="s" s="2">
+        <v>202</v>
+      </c>
+      <c r="T36" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U36" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V36" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W36" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X36" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y36" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z36" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA36" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB36" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC36" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD36" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE36" t="s" s="2">
+        <v>197</v>
+      </c>
+      <c r="AF36" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG36" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH36" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI36" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="AJ36" t="s" s="2">
+        <v>203</v>
+      </c>
+      <c r="AK36" t="s" s="2">
+        <v>204</v>
+      </c>
+      <c r="AL36" t="s" s="2">
+        <v>205</v>
+      </c>
+      <c r="AM36" t="s" s="2">
         <v>40</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AM21">
+  <autoFilter ref="A1:AM36">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -3133,7 +4833,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI20">
+  <conditionalFormatting sqref="A2:AI35">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>